<commit_message>
Lab 9 temp, with simulation error
1. Should Include .coe file for both I_MEM and D_MEM, otherwise it would have some initialization problem for those BRAM during the simulation.
2. Generated Pipeline_demo_tb.v, but still have some bugs, I'm not sure about where the bug could be, it now seems can fetch the instructions from I_MEM.
3. During the simulation, the PCx changed weird... It shows some un-decoded value, which is not what I expected.
4. The pkt_out is changed from pkt_in, but not in my expected way. I'm not sure if there are some errors for instruction input or something else...
</commit_message>
<xml_diff>
--- a/lab 9/Packet/Packet_Format.xlsx
+++ b/lab 9/Packet/Packet_Format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clint/Documents/ee533/lab 9/Packet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StepF\Documents\GitHub\ee533\lab 9\Packet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE16303-01CF-4A4B-8C63-8A80946FBB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F51B40-9A5E-4DC3-ACF9-E230D6A68005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="60">
   <si>
     <t>VER</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,10 +115,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>64 Bytes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1C 46</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,10 +139,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0000 0000 0100 0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0001 1100 0100 0110</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -254,6 +246,18 @@
   </si>
   <si>
     <t>0000 0000 0000 0000 0000 0000 0000 0000 0000 0000 0000 0000 0000 0000 0000 0001</t>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72 Bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000 0000 0100 1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -264,13 +268,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -279,7 +283,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -287,7 +291,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -497,6 +501,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,57 +534,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -836,49 +840,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="S81" sqref="S81"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
       <c r="N3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="25"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P3" s="30"/>
+      <c r="Q3" s="31"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -910,33 +914,33 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="12"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="19" t="s">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="21"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="18"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
@@ -962,29 +966,29 @@
       <c r="P6" s="11"/>
       <c r="Q6" s="12"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="21"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="18"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B8" s="10" t="s">
         <v>18</v>
       </c>
@@ -1006,112 +1010,112 @@
       <c r="P8" s="11"/>
       <c r="Q8" s="12"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B9" s="19" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="21"/>
-    </row>
-    <row r="10" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="15"/>
-    </row>
-    <row r="12" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="18"/>
+    </row>
+    <row r="10" spans="2:17" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23"/>
+    </row>
+    <row r="12" spans="2:17" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22" t="s">
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
       <c r="N13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O13" s="22" t="s">
+      <c r="O13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="23"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P13" s="19"/>
+      <c r="Q13" s="20"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B14" s="6" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20" t="s">
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
       <c r="N14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P14" s="17"/>
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1123,19 +1127,19 @@
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O15" s="11">
         <v>0</v>
@@ -1143,107 +1147,107 @@
       <c r="P15" s="11"/>
       <c r="Q15" s="12"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
       <c r="N16" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="12"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B17" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17" t="s">
+      <c r="E17" s="14"/>
+      <c r="F17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17" t="s">
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="18"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="15"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20" t="s">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20" t="s">
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="21"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="18"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B19" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
@@ -1253,23 +1257,23 @@
       <c r="P19" s="11"/>
       <c r="Q19" s="12"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B20" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -1279,53 +1283,53 @@
       <c r="P20" s="11"/>
       <c r="Q20" s="12"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="18"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="19" t="s">
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="15"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="21"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="18"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B23" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -1345,9 +1349,9 @@
       <c r="P23" s="11"/>
       <c r="Q23" s="12"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B24" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -1357,7 +1361,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -1367,49 +1371,49 @@
       <c r="P24" s="11"/>
       <c r="Q24" s="12"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="16" t="s">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B25" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="18"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="21"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="15"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B26" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="18"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B27" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -1427,9 +1431,9 @@
       <c r="P27" s="11"/>
       <c r="Q27" s="12"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B28" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -1447,9 +1451,9 @@
       <c r="P28" s="11"/>
       <c r="Q28" s="12"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B29" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -1467,9 +1471,9 @@
       <c r="P29" s="11"/>
       <c r="Q29" s="12"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B30" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -1487,9 +1491,9 @@
       <c r="P30" s="11"/>
       <c r="Q30" s="12"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B31" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
@@ -1507,9 +1511,9 @@
       <c r="P31" s="11"/>
       <c r="Q31" s="12"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B32" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -1527,9 +1531,9 @@
       <c r="P32" s="11"/>
       <c r="Q32" s="12"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B33" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -1547,9 +1551,9 @@
       <c r="P33" s="11"/>
       <c r="Q33" s="12"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B34" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -1567,9 +1571,9 @@
       <c r="P34" s="11"/>
       <c r="Q34" s="12"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B35" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -1587,9 +1591,9 @@
       <c r="P35" s="11"/>
       <c r="Q35" s="12"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B36" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -1607,9 +1611,9 @@
       <c r="P36" s="11"/>
       <c r="Q36" s="12"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B37" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -1627,92 +1631,92 @@
       <c r="P37" s="11"/>
       <c r="Q37" s="12"/>
     </row>
-    <row r="38" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="15"/>
-    </row>
-    <row r="64" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="23"/>
+    </row>
+    <row r="64" ht="14.25" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B65" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="D65" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E65" s="22"/>
-      <c r="F65" s="22" t="s">
+      <c r="E65" s="19"/>
+      <c r="F65" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
-      <c r="I65" s="22"/>
-      <c r="J65" s="22" t="s">
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K65" s="22"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="22"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
+      <c r="M65" s="19"/>
       <c r="N65" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O65" s="22" t="s">
+      <c r="O65" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="P65" s="22"/>
-      <c r="Q65" s="23"/>
-    </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P65" s="19"/>
+      <c r="Q65" s="20"/>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B66" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20" t="s">
+      <c r="E66" s="17"/>
+      <c r="F66" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="20"/>
-      <c r="H66" s="20"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="20" t="s">
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="K66" s="20"/>
-      <c r="L66" s="20"/>
-      <c r="M66" s="20"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
       <c r="N66" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O66" s="20" t="s">
+      <c r="O66" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="P66" s="20"/>
-      <c r="Q66" s="21"/>
-    </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P66" s="17"/>
+      <c r="Q66" s="18"/>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B67" s="4" t="s">
         <v>20</v>
       </c>
@@ -1724,19 +1728,19 @@
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="11" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
       <c r="J67" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
       <c r="N67" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O67" s="11">
         <v>0</v>
@@ -1744,107 +1748,107 @@
       <c r="P67" s="11"/>
       <c r="Q67" s="12"/>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B68" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="D68" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="E68" s="11"/>
       <c r="F68" s="11" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K68" s="11"/>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
       <c r="N68" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O68" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P68" s="11"/>
       <c r="Q68" s="12"/>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B69" s="16" t="s">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B69" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17" t="s">
+      <c r="C69" s="14"/>
+      <c r="D69" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17" t="s">
+      <c r="E69" s="14"/>
+      <c r="F69" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17" t="s">
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
-      <c r="M69" s="17"/>
-      <c r="N69" s="17"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
-      <c r="Q69" s="18"/>
-    </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B70" s="19" t="s">
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="14"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="14"/>
+      <c r="P69" s="14"/>
+      <c r="Q69" s="15"/>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B70" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20" t="s">
+      <c r="C70" s="17"/>
+      <c r="D70" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20" t="s">
+      <c r="E70" s="17"/>
+      <c r="F70" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G70" s="20"/>
-      <c r="H70" s="20"/>
-      <c r="I70" s="20"/>
-      <c r="J70" s="20" t="s">
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+      <c r="J70" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K70" s="20"/>
-      <c r="L70" s="20"/>
-      <c r="M70" s="20"/>
-      <c r="N70" s="20"/>
-      <c r="O70" s="20"/>
-      <c r="P70" s="20"/>
-      <c r="Q70" s="21"/>
-    </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
+      <c r="Q70" s="18"/>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B71" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E71" s="11"/>
       <c r="F71" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
       <c r="J71" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K71" s="11"/>
       <c r="L71" s="11"/>
@@ -1854,23 +1858,23 @@
       <c r="P71" s="11"/>
       <c r="Q71" s="12"/>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B72" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
       <c r="J72" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K72" s="11"/>
       <c r="L72" s="11"/>
@@ -1880,53 +1884,53 @@
       <c r="P72" s="11"/>
       <c r="Q72" s="12"/>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B73" s="16" t="s">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B73" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17" t="s">
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="18"/>
-    </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B74" s="19" t="s">
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="14"/>
+      <c r="Q73" s="15"/>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B74" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="20"/>
-      <c r="H74" s="20"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="20" t="s">
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+      <c r="J74" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K74" s="20"/>
-      <c r="L74" s="20"/>
-      <c r="M74" s="20"/>
-      <c r="N74" s="20"/>
-      <c r="O74" s="20"/>
-      <c r="P74" s="20"/>
-      <c r="Q74" s="21"/>
-    </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K74" s="17"/>
+      <c r="L74" s="17"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="18"/>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B75" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -1946,9 +1950,9 @@
       <c r="P75" s="11"/>
       <c r="Q75" s="12"/>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B76" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -1958,7 +1962,7 @@
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
       <c r="J76" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K76" s="11"/>
       <c r="L76" s="11"/>
@@ -1968,49 +1972,49 @@
       <c r="P76" s="11"/>
       <c r="Q76" s="12"/>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B77" s="16" t="s">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B77" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="17"/>
-      <c r="J77" s="17"/>
-      <c r="K77" s="17"/>
-      <c r="L77" s="17"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="18"/>
-    </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B78" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="20"/>
-      <c r="H78" s="20"/>
-      <c r="I78" s="20"/>
-      <c r="J78" s="20"/>
-      <c r="K78" s="20"/>
-      <c r="L78" s="20"/>
-      <c r="M78" s="20"/>
-      <c r="N78" s="20"/>
-      <c r="O78" s="20"/>
-      <c r="P78" s="20"/>
-      <c r="Q78" s="21"/>
-    </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+      <c r="Q77" s="15"/>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B78" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+      <c r="J78" s="17"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="18"/>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B79" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -2028,9 +2032,9 @@
       <c r="P79" s="11"/>
       <c r="Q79" s="12"/>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B80" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
@@ -2048,9 +2052,9 @@
       <c r="P80" s="11"/>
       <c r="Q80" s="12"/>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B81" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
@@ -2068,9 +2072,9 @@
       <c r="P81" s="11"/>
       <c r="Q81" s="12"/>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B82" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
@@ -2088,9 +2092,9 @@
       <c r="P82" s="11"/>
       <c r="Q82" s="12"/>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B83" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
@@ -2108,9 +2112,9 @@
       <c r="P83" s="11"/>
       <c r="Q83" s="12"/>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B84" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
@@ -2128,9 +2132,9 @@
       <c r="P84" s="11"/>
       <c r="Q84" s="12"/>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B85" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
@@ -2148,9 +2152,9 @@
       <c r="P85" s="11"/>
       <c r="Q85" s="12"/>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B86" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
@@ -2168,9 +2172,9 @@
       <c r="P86" s="11"/>
       <c r="Q86" s="12"/>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B87" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
@@ -2188,9 +2192,9 @@
       <c r="P87" s="11"/>
       <c r="Q87" s="12"/>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B88" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
@@ -2208,48 +2212,56 @@
       <c r="P88" s="11"/>
       <c r="Q88" s="12"/>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B89" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C89" s="26"/>
-      <c r="D89" s="26"/>
-      <c r="E89" s="26"/>
-      <c r="F89" s="26"/>
-      <c r="G89" s="26"/>
-      <c r="H89" s="26"/>
-      <c r="I89" s="26"/>
-      <c r="J89" s="26"/>
-      <c r="K89" s="26"/>
-      <c r="L89" s="26"/>
-      <c r="M89" s="26"/>
-      <c r="N89" s="26"/>
-      <c r="O89" s="26"/>
-      <c r="P89" s="26"/>
-      <c r="Q89" s="28"/>
-    </row>
-    <row r="90" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C90" s="30"/>
-      <c r="D90" s="30"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="30"/>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="30"/>
-      <c r="L90" s="30"/>
-      <c r="M90" s="30"/>
-      <c r="N90" s="30"/>
-      <c r="O90" s="30"/>
-      <c r="P90" s="30"/>
-      <c r="Q90" s="31"/>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="B89" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="25"/>
+      <c r="G89" s="25"/>
+      <c r="H89" s="25"/>
+      <c r="I89" s="25"/>
+      <c r="J89" s="25"/>
+      <c r="K89" s="25"/>
+      <c r="L89" s="25"/>
+      <c r="M89" s="25"/>
+      <c r="N89" s="25"/>
+      <c r="O89" s="25"/>
+      <c r="P89" s="25"/>
+      <c r="Q89" s="26"/>
+    </row>
+    <row r="90" spans="2:17" ht="14.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B90" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="28"/>
+      <c r="J90" s="28"/>
+      <c r="K90" s="28"/>
+      <c r="L90" s="28"/>
+      <c r="M90" s="28"/>
+      <c r="N90" s="28"/>
+      <c r="O90" s="28"/>
+      <c r="P90" s="28"/>
+      <c r="Q90" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="130">
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:Q5"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J19:Q19"/>
     <mergeCell ref="B89:Q89"/>
     <mergeCell ref="B90:Q90"/>
     <mergeCell ref="D3:E3"/>
@@ -2270,19 +2282,6 @@
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:Q5"/>
-    <mergeCell ref="B9:Q9"/>
-    <mergeCell ref="B10:Q10"/>
-    <mergeCell ref="J20:Q20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="J17:Q17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="J18:Q18"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:I13"/>
     <mergeCell ref="J13:M13"/>
@@ -2295,10 +2294,6 @@
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="J19:Q19"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="J21:Q21"/>
     <mergeCell ref="B23:I23"/>
@@ -2314,6 +2309,15 @@
     <mergeCell ref="B25:Q25"/>
     <mergeCell ref="B22:I22"/>
     <mergeCell ref="J22:Q22"/>
+    <mergeCell ref="J20:Q20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="J17:Q17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="J18:Q18"/>
     <mergeCell ref="B28:Q28"/>
     <mergeCell ref="B32:Q32"/>
     <mergeCell ref="B34:Q34"/>

</xml_diff>